<commit_message>
Added Browse for file activity to allow user to select the input file - addresses requirement that input file can land in a random folder, and user chooses the file. Removed unused / commented out activities.
</commit_message>
<xml_diff>
--- a/Data/Output/Results.xlsx
+++ b/Data/Output/Results.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <x:si>
     <x:t>Postcode</x:t>
   </x:si>
@@ -51,33 +51,6 @@
   </x:si>
   <x:si>
     <x:t>Postcode is invalid.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0300</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0500</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7000</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9100</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7800</x:t>
-  </x:si>
-  <x:si>
-    <x:t>abc</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Business Exception</x:t>
-  </x:si>
-  <x:si>
-    <x:t>340!</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3004</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -451,70 +424,14 @@
         <x:v>6</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <x:c r="A5" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <x:c r="A6" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <x:c r="A7" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <x:c r="A8" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B8" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <x:c r="A9" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="B9" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <x:c r="A10" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B10" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <x:c r="A11" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="B11" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <x:c r="A12" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="B12" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
+    <x:row r="5" spans="1:2" x14ac:dyDescent="0.2"/>
+    <x:row r="6" spans="1:2" x14ac:dyDescent="0.2"/>
+    <x:row r="7" spans="1:2" x14ac:dyDescent="0.2"/>
+    <x:row r="8" spans="1:2" x14ac:dyDescent="0.2"/>
+    <x:row r="9" spans="1:2" x14ac:dyDescent="0.2"/>
+    <x:row r="10" spans="1:2" x14ac:dyDescent="0.2"/>
+    <x:row r="11" spans="1:2" x14ac:dyDescent="0.2"/>
+    <x:row r="12" spans="1:2" x14ac:dyDescent="0.2"/>
     <x:row r="13" spans="1:2"/>
     <x:row r="14" spans="1:2"/>
   </x:sheetData>

</xml_diff>